<commit_message>
Moderator not paid error fixed
</commit_message>
<xml_diff>
--- a/QA Report/IMS-002 - Bug Report.xlsx
+++ b/QA Report/IMS-002 - Bug Report.xlsx
@@ -110,9 +110,6 @@
     <t>Add some data validations for exams.php</t>
   </si>
   <si>
-    <t>when enters existing username and name</t>
-  </si>
-  <si>
     <t>Data inserted to database and got a success popup</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>when enters existing username and another name</t>
   </si>
 </sst>
 </file>
@@ -222,17 +222,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,7 +517,7 @@
   <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,34 +532,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -590,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>13</v>
@@ -613,15 +613,15 @@
         <v>22</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="9" t="s">
-        <v>34</v>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>14</v>
@@ -646,7 +646,7 @@
       <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -656,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>14</v>
@@ -679,7 +679,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -689,7 +689,7 @@
         <v>12</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>14</v>
@@ -700,19 +700,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="3"/>
@@ -720,7 +720,7 @@
         <v>12</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Date Validations added to newStudent.php | QA Report updated
</commit_message>
<xml_diff>
--- a/QA Report/IMS-002 - Bug Report.xlsx
+++ b/QA Report/IMS-002 - Bug Report.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,8 +646,8 @@
       <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>15</v>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Data validations added to exams.php | QA Report updated
</commit_message>
<xml_diff>
--- a/QA Report/IMS-002 - Bug Report.xlsx
+++ b/QA Report/IMS-002 - Bug Report.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,8 +679,8 @@
         <v>26</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="8" t="s">
-        <v>15</v>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Finals: Project development 100% done. | Final test canceled. QA 3rd stage canceled!
</commit_message>
<xml_diff>
--- a/QA Report/IMS-002 - Bug Report.xlsx
+++ b/QA Report/IMS-002 - Bug Report.xlsx
@@ -71,9 +71,6 @@
     <t>26.01.2023</t>
   </si>
   <si>
-    <t>not finishd</t>
-  </si>
-  <si>
     <t>Case</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>when enters existing username and another name</t>
+  </si>
+  <si>
+    <t>Optional</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,14 +225,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,7 +517,7 @@
   <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,41 +532,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -590,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>13</v>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -610,18 +610,18 @@
         <v>10</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>14</v>
@@ -632,31 +632,31 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>14</v>
@@ -667,29 +667,29 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>14</v>
@@ -700,27 +700,27 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>

</xml_diff>